<commit_message>
Add more Font led7seg, Wiring EagleCad
</commit_message>
<xml_diff>
--- a/document/Button_Calculate.xlsx
+++ b/document/Button_Calculate.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Button" sheetId="1" r:id="rId1"/>
+    <sheet name="Led7Seg" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -56,7 +57,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -74,12 +75,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,9 +102,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -379,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +404,7 @@
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -438,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -459,7 +472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -480,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -501,7 +514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -522,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -543,7 +556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -564,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -585,7 +598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -603,7 +616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -620,7 +633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -640,8 +653,12 @@
         <f t="shared" ref="O14" si="2">O15-3</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14" t="str">
+        <f>DEC2HEX(M14)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -661,8 +678,12 @@
         <f t="shared" ref="O15" si="3">O16-3</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15" t="str">
+        <f t="shared" ref="Q15:Q23" si="4">DEC2HEX(M15)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -679,11 +700,15 @@
         <v>128</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16:O21" si="4">O17-3</f>
+        <f t="shared" ref="O16:O21" si="5">O17-3</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" t="str">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -700,11 +725,15 @@
         <v>1024</v>
       </c>
       <c r="O17">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="Q17" t="str">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -721,11 +750,15 @@
         <v>8192</v>
       </c>
       <c r="O18">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Q18" t="str">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -742,11 +775,15 @@
         <v>65536</v>
       </c>
       <c r="O19">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="Q19" t="str">
         <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -759,15 +796,22 @@
       <c r="I20">
         <v>10</v>
       </c>
+      <c r="L20">
+        <v>524288</v>
+      </c>
       <c r="M20">
         <v>524088</v>
       </c>
       <c r="O20">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Q20" t="str">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7FF38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -784,11 +828,15 @@
         <v>4194304</v>
       </c>
       <c r="O21">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="Q21" t="str">
         <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>16</v>
       </c>
@@ -799,11 +847,15 @@
         <v>33554432</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="O22" si="5">O23-3</f>
+        <f t="shared" ref="O22" si="6">O23-3</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" t="str">
+        <f t="shared" si="4"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>17</v>
       </c>
@@ -815,6 +867,96 @@
       </c>
       <c r="O23">
         <v>29</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="4"/>
+        <v>10000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
+        <v>11111111</v>
+      </c>
+      <c r="E2" s="2">
+        <f>BIN2DEC(C2)</f>
+        <v>255</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>BIN2HEX(C2,)</f>
+        <v>FF</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="str">
+        <f>E10&amp;C7&amp;B6&amp;B8&amp;C9&amp;D8&amp;D6&amp;C5</f>
+        <v>01010000</v>
+      </c>
+      <c r="E3" s="2">
+        <f>BIN2DEC(C3)</f>
+        <v>80</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>BIN2HEX(C3,)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>